<commit_message>
small changes in control file M2.1
</commit_message>
<xml_diff>
--- a/IO_M2.1/RunControl_M2.1.xlsx
+++ b/IO_M2.1/RunControl_M2.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1211,7 +1211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,16 +1226,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1735,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B108" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
@@ -1911,59 +1911,59 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="30"/>
+      <c r="F4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="30" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="30" t="s">
+      <c r="K4" s="33"/>
+      <c r="L4" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="31" t="s">
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="29" t="s">
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="32" t="s">
+      <c r="Z4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="29" t="s">
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
       <c r="AF4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1971,12 +1971,12 @@
       <c r="AH4" s="22"/>
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
-      <c r="AK4" s="33" t="s">
+      <c r="AK4" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="AL4" s="33"/>
-      <c r="AM4" s="33"/>
-      <c r="AN4" s="33"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="35"/>
+      <c r="AN4" s="35"/>
       <c r="AO4" s="16"/>
       <c r="AP4" s="23"/>
       <c r="AQ4" s="21"/>
@@ -12768,17 +12768,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AK4:AN4"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI11 AI47:AI51 AI27:AI36 AI13:AI25 AI65:AI69 AI53:AI57 AI59:AI63 AI38:AI45 AI74:AI79 AI95:AI104 AI81:AI93">
@@ -13356,10 +13356,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E13"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13442,6 +13442,12 @@
         <v>2.6999999999999996E-2</v>
       </c>
     </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>0.14^2</f>
+        <v>1.9600000000000003E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>